<commit_message>
Add eMember menu management features and refactor components
- Implemented server actions to fetch eMember menus and user guides with error handling.
- Created EmMenuPage component to display eMember menus with loading states and integrated MenuTables for data presentation.
- Removed obsolete components to streamline the codebase.
- Updated database schema with new entries for eMember functionalities.
</commit_message>
<xml_diff>
--- a/settings/Seed Data.xlsx
+++ b/settings/Seed Data.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XSP Project\xps-master-by-jk\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7FA0F5-2E11-484A-AA87-3CFD06627858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85FBF35-8B1E-4794-8E21-DC31C61AAD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Xps User Guide" sheetId="5" r:id="rId1"/>
+    <sheet name="eMember Menu" sheetId="11" r:id="rId1"/>
     <sheet name="Enum" sheetId="19" r:id="rId2"/>
     <sheet name="Portals" sheetId="17" r:id="rId3"/>
     <sheet name="Users" sheetId="18" r:id="rId4"/>
     <sheet name="Xps Menu" sheetId="6" r:id="rId5"/>
     <sheet name="Xps Menu Descriptions" sheetId="4" r:id="rId6"/>
-    <sheet name="Xps Tables" sheetId="3" r:id="rId7"/>
-    <sheet name="Xps Columns" sheetId="8" r:id="rId8"/>
-    <sheet name="Xps Test Cases" sheetId="7" r:id="rId9"/>
-    <sheet name="Xps Bugs" sheetId="9" r:id="rId10"/>
-    <sheet name="Xps Released Task" sheetId="10" r:id="rId11"/>
-    <sheet name="eMember Menu" sheetId="11" r:id="rId12"/>
+    <sheet name="Xps User Guide" sheetId="5" r:id="rId7"/>
+    <sheet name="Xps Tables" sheetId="3" r:id="rId8"/>
+    <sheet name="Xps Columns" sheetId="8" r:id="rId9"/>
+    <sheet name="Xps Test Cases" sheetId="7" r:id="rId10"/>
+    <sheet name="Xps Bugs" sheetId="9" r:id="rId11"/>
+    <sheet name="Xps Released Task" sheetId="10" r:id="rId12"/>
     <sheet name="eMember Menu Desc" sheetId="12" r:id="rId13"/>
     <sheet name="eMember User Guide" sheetId="1" r:id="rId14"/>
     <sheet name="eMember Tables" sheetId="2" r:id="rId15"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="151">
   <si>
     <t>emChapterNo</t>
   </si>
@@ -929,152 +929,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA71A04-11EA-4D0B-B6D2-7FD344989619}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F88E74-BD67-42CE-B055-DDE648DF10E9}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FF00B0F0"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1"/>
-    <col min="2" max="2" width="28.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="1"/>
-    <col min="4" max="16384" width="16.140625" style="3"/>
+    <col min="1" max="1" width="23.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>17</v>
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="str">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>EWIH</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="str">
-        <f t="shared" ref="B4:B11" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>ZGUD</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="str">
+        <v>FLOG</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="str">
+        <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
+        <v>YLOK</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JGTO</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="str">
+        <v>PRKZ</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>UXFC</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="str">
+        <v>LMZP</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WFTK</v>
-      </c>
-      <c r="C7" s="1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="str">
+        <v>DPXH</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ZKDL</v>
-      </c>
-      <c r="C8" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="str">
+        <v>RFXI</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>GLNQ</v>
-      </c>
-      <c r="C9" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>DMUL</v>
-      </c>
-      <c r="C10" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>GVRM</v>
-      </c>
-      <c r="C11" s="1">
-        <v>9</v>
+        <v>MPSF</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
+        <v>VDXV</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1083,6 +1075,73 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DA93E-1B9C-4113-B4A9-8115F889330E}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A989FAC-8575-4264-86E5-883569E54F3F}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1141,7 +1200,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBFE0B6-E602-4629-B2D2-1D3D79579B76}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1193,45 +1252,6 @@
       </c>
       <c r="I1" s="7" t="s">
         <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F88E74-BD67-42CE-B055-DDE648DF10E9}">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1573,7 +1593,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H6"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2231,7 +2251,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2278,7 +2298,7 @@
     <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>ZKBF</v>
+        <v>SOQB</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>80</v>
@@ -2293,7 +2313,7 @@
     <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>DZEX</v>
+        <v>LMAI</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>81</v>
@@ -2308,7 +2328,7 @@
     <row r="5" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>OBRW</v>
+        <v>HHYV</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
@@ -2323,7 +2343,7 @@
     <row r="6" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>OMWA</v>
+        <v>QGXD</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>80</v>
@@ -2338,7 +2358,7 @@
     <row r="7" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KEEN</v>
+        <v>ZNDA</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>81</v>
@@ -2353,7 +2373,7 @@
     <row r="8" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>UTUK</v>
+        <v>VJQT</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -2368,7 +2388,7 @@
     <row r="9" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>UEYV</v>
+        <v>STDQ</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>80</v>
@@ -2383,7 +2403,7 @@
     <row r="10" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>TVRT</v>
+        <v>KUAZ</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>81</v>
@@ -2431,6 +2451,160 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA71A04-11EA-4D0B-B6D2-7FD344989619}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" style="1"/>
+    <col min="2" max="2" width="28.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="1"/>
+    <col min="4" max="16384" width="16.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
+        <v>ZKDB</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="str">
+        <f t="shared" ref="B4:B11" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
+        <v>ZSNT</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>HVPV</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>SZID</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>GCWP</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>BXQU</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>RXNJ</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>WKWC</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>INMB</v>
+      </c>
+      <c r="C11" s="1">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD2043-75FB-4D5F-9033-C3F3EE0DCB0F}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2462,7 +2636,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7EC624-B5B6-46EE-84B1-DF9F4080EB6C}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2496,71 +2670,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DA93E-1B9C-4113-B4A9-8115F889330E}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement XPS tables management features and refactor components
- Added server actions to fetch all XPS tables and individual XPS table details with error handling.
- Updated XPSTablesPage component to display a list of XPS tables with loading states and integrated DbTables for data presentation.
- Enhanced XpsColumnsPage component to show columns of a specific XPS table, including loading indicators and error handling.
- Removed obsolete components related to filtering and columns to streamline the codebase.
- Updated database schema with new entries for XPS functionalities.
</commit_message>
<xml_diff>
--- a/settings/Seed Data.xlsx
+++ b/settings/Seed Data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XSP Project\xps-master-by-jk\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F85FBF35-8B1E-4794-8E21-DC31C61AAD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461B16B4-F31D-40A8-B4B9-E565AF00DD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="eMember Menu" sheetId="11" r:id="rId1"/>
+    <sheet name="Xps Columns" sheetId="8" r:id="rId1"/>
     <sheet name="Enum" sheetId="19" r:id="rId2"/>
     <sheet name="Portals" sheetId="17" r:id="rId3"/>
     <sheet name="Users" sheetId="18" r:id="rId4"/>
@@ -21,10 +21,10 @@
     <sheet name="Xps Menu Descriptions" sheetId="4" r:id="rId6"/>
     <sheet name="Xps User Guide" sheetId="5" r:id="rId7"/>
     <sheet name="Xps Tables" sheetId="3" r:id="rId8"/>
-    <sheet name="Xps Columns" sheetId="8" r:id="rId9"/>
-    <sheet name="Xps Test Cases" sheetId="7" r:id="rId10"/>
-    <sheet name="Xps Bugs" sheetId="9" r:id="rId11"/>
-    <sheet name="Xps Released Task" sheetId="10" r:id="rId12"/>
+    <sheet name="Xps Test Cases" sheetId="7" r:id="rId9"/>
+    <sheet name="Xps Bugs" sheetId="9" r:id="rId10"/>
+    <sheet name="Xps Released Task" sheetId="10" r:id="rId11"/>
+    <sheet name="eMember Menu" sheetId="11" r:id="rId12"/>
     <sheet name="eMember Menu Desc" sheetId="12" r:id="rId13"/>
     <sheet name="eMember User Guide" sheetId="1" r:id="rId14"/>
     <sheet name="eMember Tables" sheetId="2" r:id="rId15"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="155">
   <si>
     <t>emChapterNo</t>
   </si>
@@ -510,6 +510,18 @@
   </si>
   <si>
     <t>XX12P28</t>
+  </si>
+  <si>
+    <t>Another table</t>
+  </si>
+  <si>
+    <t>Next table</t>
+  </si>
+  <si>
+    <t>Deomo Col</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -929,144 +941,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F88E74-BD67-42CE-B055-DDE648DF10E9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7EC624-B5B6-46EE-84B1-DF9F4080EB6C}">
   <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
+    <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="str">
-        <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>FLOG</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="str">
-        <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>YLOK</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>PRKZ</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>LMZP</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>DPXH</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>RFXI</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>MPSF</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="str">
-        <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>VDXV</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>110</v>
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1075,73 +996,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DA93E-1B9C-4113-B4A9-8115F889330E}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A989FAC-8575-4264-86E5-883569E54F3F}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1200,7 +1054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBFE0B6-E602-4629-B2D2-1D3D79579B76}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1252,6 +1106,152 @@
       </c>
       <c r="I1" s="7" t="s">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F88E74-BD67-42CE-B055-DDE648DF10E9}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
+        <v>DYFX</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="str">
+        <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
+        <v>RBGG</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>QIUN</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>QUAX</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>UBLI</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>HBKX</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>QEXM</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="str">
+        <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
+        <v>UCCX</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2298,7 +2298,7 @@
     <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>SOQB</v>
+        <v>WEEI</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>80</v>
@@ -2313,7 +2313,7 @@
     <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>LMAI</v>
+        <v>JAZN</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>81</v>
@@ -2328,7 +2328,7 @@
     <row r="5" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>HHYV</v>
+        <v>VYXY</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
@@ -2343,7 +2343,7 @@
     <row r="6" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>QGXD</v>
+        <v>ZHJD</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>80</v>
@@ -2358,7 +2358,7 @@
     <row r="7" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ZNDA</v>
+        <v>USYH</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>81</v>
@@ -2373,7 +2373,7 @@
     <row r="8" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>VJQT</v>
+        <v>GEGM</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -2388,7 +2388,7 @@
     <row r="9" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>STDQ</v>
+        <v>ZODY</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>80</v>
@@ -2403,7 +2403,7 @@
     <row r="10" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>KUAZ</v>
+        <v>QBUT</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>81</v>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="B3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>ZKDB</v>
+        <v>BKGK</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f t="shared" ref="B4:B11" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>ZSNT</v>
+        <v>UAMA</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>HVPV</v>
+        <v>SQGE</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -2533,7 +2533,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SZID</v>
+        <v>JBCX</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -2545,7 +2545,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>GCWP</v>
+        <v>JQJA</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>BXQU</v>
+        <v>MWGG</v>
       </c>
       <c r="C8" s="1">
         <v>7</v>
@@ -2569,7 +2569,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>RXNJ</v>
+        <v>IFQO</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WKWC</v>
+        <v>DDRA</v>
       </c>
       <c r="C10" s="1">
         <v>9</v>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>INMB</v>
+        <v>IVSZ</v>
       </c>
       <c r="C11" s="1">
         <v>9</v>
@@ -2609,10 +2609,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K14:K15"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2628,7 +2628,12 @@
     </row>
     <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2637,34 +2642,65 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7EC624-B5B6-46EE-84B1-DF9F4080EB6C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DA93E-1B9C-4113-B4A9-8115F889330E}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>24</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add eMember tables management features and refactor components
- Implemented server actions to fetch eMember tables with error handling.
- Created EmTablesPage component to display eMember tables with loading states and integrated EmDbTables for data presentation.
- Removed obsolete components related to filtering and columns to streamline the codebase.
- Updated database schema with new entries for eMember functionalities.
</commit_message>
<xml_diff>
--- a/settings/Seed Data.xlsx
+++ b/settings/Seed Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XSP Project\xps-master-by-jk\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{461B16B4-F31D-40A8-B4B9-E565AF00DD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452A438B-5030-46EA-A3E0-80B8A5068C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -948,7 +948,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactor XPS columns page to fetch and display table columns
- Updated the XpsColumnsPage component to retrieve and display columns for a specific XPS table, including loading states and error handling.
- Changed the data fetching logic to include emColumns instead of emMenu for accurate data representation.
- Enhanced the UI with a table structure to present column names clearly.
- Renamed the component from EmColumnsPage to XpsColumnsPage for consistency with naming conventions.
</commit_message>
<xml_diff>
--- a/settings/Seed Data.xlsx
+++ b/settings/Seed Data.xlsx
@@ -8,27 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XSP Project\xps-master-by-jk\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452A438B-5030-46EA-A3E0-80B8A5068C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E3509C-224A-4030-B0D6-E444DD89675B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Xps Columns" sheetId="8" r:id="rId1"/>
-    <sheet name="Enum" sheetId="19" r:id="rId2"/>
-    <sheet name="Portals" sheetId="17" r:id="rId3"/>
-    <sheet name="Users" sheetId="18" r:id="rId4"/>
-    <sheet name="Xps Menu" sheetId="6" r:id="rId5"/>
-    <sheet name="Xps Menu Descriptions" sheetId="4" r:id="rId6"/>
-    <sheet name="Xps User Guide" sheetId="5" r:id="rId7"/>
-    <sheet name="Xps Tables" sheetId="3" r:id="rId8"/>
-    <sheet name="Xps Test Cases" sheetId="7" r:id="rId9"/>
-    <sheet name="Xps Bugs" sheetId="9" r:id="rId10"/>
-    <sheet name="Xps Released Task" sheetId="10" r:id="rId11"/>
-    <sheet name="eMember Menu" sheetId="11" r:id="rId12"/>
-    <sheet name="eMember Menu Desc" sheetId="12" r:id="rId13"/>
-    <sheet name="eMember User Guide" sheetId="1" r:id="rId14"/>
-    <sheet name="eMember Tables" sheetId="2" r:id="rId15"/>
-    <sheet name="eMember Columns" sheetId="13" r:id="rId16"/>
+    <sheet name="eMember Columns" sheetId="13" r:id="rId1"/>
+    <sheet name="eMember Tables" sheetId="2" r:id="rId2"/>
+    <sheet name="Enum" sheetId="19" r:id="rId3"/>
+    <sheet name="Portals" sheetId="17" r:id="rId4"/>
+    <sheet name="Users" sheetId="18" r:id="rId5"/>
+    <sheet name="Xps Menu" sheetId="6" r:id="rId6"/>
+    <sheet name="Xps Menu Descriptions" sheetId="4" r:id="rId7"/>
+    <sheet name="Xps User Guide" sheetId="5" r:id="rId8"/>
+    <sheet name="Xps Tables" sheetId="3" r:id="rId9"/>
+    <sheet name="Xps Columns" sheetId="8" r:id="rId10"/>
+    <sheet name="Xps Test Cases" sheetId="7" r:id="rId11"/>
+    <sheet name="Xps Bugs" sheetId="9" r:id="rId12"/>
+    <sheet name="Xps Released Task" sheetId="10" r:id="rId13"/>
+    <sheet name="eMember Menu" sheetId="11" r:id="rId14"/>
+    <sheet name="eMember Menu Desc" sheetId="12" r:id="rId15"/>
+    <sheet name="eMember User Guide" sheetId="1" r:id="rId16"/>
     <sheet name="eMember Test Cases" sheetId="14" r:id="rId17"/>
     <sheet name="eMember Bugs" sheetId="15" r:id="rId18"/>
     <sheet name="eMember Released Task" sheetId="16" r:id="rId19"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="158">
   <si>
     <t>emChapterNo</t>
   </si>
@@ -522,6 +522,15 @@
   </si>
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>Demo Col</t>
+  </si>
+  <si>
+    <t>Test Table 2</t>
+  </si>
+  <si>
+    <t>Test Table 3</t>
   </si>
 </sst>
 </file>
@@ -941,14 +950,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CE00FC-F1BA-4EE1-A3DF-8AB843E09614}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7EC624-B5B6-46EE-84B1-DF9F4080EB6C}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -995,7 +1067,74 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DA93E-1B9C-4113-B4A9-8115F889330E}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A989FAC-8575-4264-86E5-883569E54F3F}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1054,7 +1193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBFE0B6-E602-4629-B2D2-1D3D79579B76}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1113,7 +1252,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F88E74-BD67-42CE-B055-DDE648DF10E9}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -1161,7 +1300,7 @@
     <row r="3" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>DYFX</v>
+        <v>YWHS</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>75</v>
@@ -1173,7 +1312,7 @@
     <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>RBGG</v>
+        <v>CWLA</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>78</v>
@@ -1185,7 +1324,7 @@
     <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>QIUN</v>
+        <v>YLCP</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>76</v>
@@ -1197,7 +1336,7 @@
     <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>QUAX</v>
+        <v>PAMS</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>75</v>
@@ -1209,7 +1348,7 @@
     <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>UBLI</v>
+        <v>XXOL</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>78</v>
@@ -1221,7 +1360,7 @@
     <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>HBKX</v>
+        <v>CYAX</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>76</v>
@@ -1233,7 +1372,7 @@
     <row r="9" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>QEXM</v>
+        <v>XUWB</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>75</v>
@@ -1245,7 +1384,7 @@
     <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>UCCX</v>
+        <v>UKBZ</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>78</v>
@@ -1259,7 +1398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DB385F-AA7A-4B07-8986-C7BC0E547E48}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -1289,7 +1428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -1340,76 +1479,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476F5C88-0CAA-4005-9A01-27383EE413C1}">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.42578125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CE00FC-F1BA-4EE1-A3DF-8AB843E09614}">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1586,6 +1655,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476F5C88-0CAA-4005-9A01-27383EE413C1}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052181FB-1E4F-4A1E-B12D-45458B6E9387}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -1792,7 +1900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBF7BFE-850B-4F98-B614-3DDD73343798}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -1894,7 +2002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E09210A-B3C7-4006-9111-ED419D27687A}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2243,7 +2351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14030B2-06E1-4909-9E18-47749C3436A8}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2298,7 +2406,7 @@
     <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>WEEI</v>
+        <v>TWJG</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>80</v>
@@ -2313,7 +2421,7 @@
     <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>JAZN</v>
+        <v>RRMI</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>81</v>
@@ -2328,7 +2436,7 @@
     <row r="5" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>VYXY</v>
+        <v>WAUB</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
@@ -2343,7 +2451,7 @@
     <row r="6" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ZHJD</v>
+        <v>ROKK</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>80</v>
@@ -2358,7 +2466,7 @@
     <row r="7" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>USYH</v>
+        <v>KDOI</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>81</v>
@@ -2373,7 +2481,7 @@
     <row r="8" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>GEGM</v>
+        <v>EWBX</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -2388,7 +2496,7 @@
     <row r="9" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ZODY</v>
+        <v>TOHJ</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>80</v>
@@ -2403,7 +2511,7 @@
     <row r="10" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>QBUT</v>
+        <v>WZGI</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>81</v>
@@ -2420,7 +2528,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA7453C-C911-4FD1-9109-F66FBE59E42C}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2450,7 +2558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA71A04-11EA-4D0B-B6D2-7FD344989619}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2497,7 +2605,7 @@
       </c>
       <c r="B3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>BKGK</v>
+        <v>LASS</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -2509,7 +2617,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f t="shared" ref="B4:B11" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>UAMA</v>
+        <v>NJRA</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -2521,7 +2629,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SQGE</v>
+        <v>JKKS</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -2533,7 +2641,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JBCX</v>
+        <v>KFDC</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -2545,7 +2653,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JQJA</v>
+        <v>NRVY</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -2557,7 +2665,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>MWGG</v>
+        <v>SCJM</v>
       </c>
       <c r="C8" s="1">
         <v>7</v>
@@ -2569,7 +2677,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>IFQO</v>
+        <v>HYBB</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
@@ -2581,7 +2689,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DDRA</v>
+        <v>DBCT</v>
       </c>
       <c r="C10" s="1">
         <v>9</v>
@@ -2593,7 +2701,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>IVSZ</v>
+        <v>LWFE</v>
       </c>
       <c r="C11" s="1">
         <v>9</v>
@@ -2604,7 +2712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD2043-75FB-4D5F-9033-C3F3EE0DCB0F}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2639,71 +2747,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DA93E-1B9C-4113-B4A9-8115F889330E}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add XPS test cases management features and refactor components
- Introduced server actions to fetch XPS test cases with error handling.
- Created XpsTestCasesPage component to display test cases with loading states and integrated TestCasesTables for data presentation.
- Added filtering capabilities with XpsTCFilter component for enhanced user experience.
- Removed obsolete components related to test cases to streamline the codebase.
- Updated database schema by dropping the menuName column from the XpsTestCases model.
</commit_message>
<xml_diff>
--- a/settings/Seed Data.xlsx
+++ b/settings/Seed Data.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XSP Project\xps-master-by-jk\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E3509C-224A-4030-B0D6-E444DD89675B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1059208A-7854-4702-9B99-11AB66C73732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="eMember Columns" sheetId="13" r:id="rId1"/>
-    <sheet name="eMember Tables" sheetId="2" r:id="rId2"/>
-    <sheet name="Enum" sheetId="19" r:id="rId3"/>
-    <sheet name="Portals" sheetId="17" r:id="rId4"/>
-    <sheet name="Users" sheetId="18" r:id="rId5"/>
-    <sheet name="Xps Menu" sheetId="6" r:id="rId6"/>
-    <sheet name="Xps Menu Descriptions" sheetId="4" r:id="rId7"/>
-    <sheet name="Xps User Guide" sheetId="5" r:id="rId8"/>
-    <sheet name="Xps Tables" sheetId="3" r:id="rId9"/>
-    <sheet name="Xps Columns" sheetId="8" r:id="rId10"/>
-    <sheet name="Xps Test Cases" sheetId="7" r:id="rId11"/>
+    <sheet name="Xps Test Cases" sheetId="7" r:id="rId1"/>
+    <sheet name="eMember Columns" sheetId="13" r:id="rId2"/>
+    <sheet name="eMember Tables" sheetId="2" r:id="rId3"/>
+    <sheet name="Enum" sheetId="19" r:id="rId4"/>
+    <sheet name="Portals" sheetId="17" r:id="rId5"/>
+    <sheet name="Users" sheetId="18" r:id="rId6"/>
+    <sheet name="Xps Menu" sheetId="6" r:id="rId7"/>
+    <sheet name="Xps Menu Descriptions" sheetId="4" r:id="rId8"/>
+    <sheet name="Xps User Guide" sheetId="5" r:id="rId9"/>
+    <sheet name="Xps Tables" sheetId="3" r:id="rId10"/>
+    <sheet name="Xps Columns" sheetId="8" r:id="rId11"/>
     <sheet name="Xps Bugs" sheetId="9" r:id="rId12"/>
     <sheet name="Xps Released Task" sheetId="10" r:id="rId13"/>
     <sheet name="eMember Menu" sheetId="11" r:id="rId14"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="164">
   <si>
     <t>emChapterNo</t>
   </si>
@@ -531,6 +531,24 @@
   </si>
   <si>
     <t>Test Table 3</t>
+  </si>
+  <si>
+    <t>TL01</t>
+  </si>
+  <si>
+    <t>Verify my name</t>
+  </si>
+  <si>
+    <t>TL02</t>
+  </si>
+  <si>
+    <t>TL03</t>
+  </si>
+  <si>
+    <t>TL04</t>
+  </si>
+  <si>
+    <t>TL05</t>
   </si>
 </sst>
 </file>
@@ -950,61 +968,214 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CE00FC-F1BA-4EE1-A3DF-8AB843E09614}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DA93E-1B9C-4113-B4A9-8115F889330E}">
   <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
+    <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="J5" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="10">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD2043-75FB-4D5F-9033-C3F3EE0DCB0F}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1012,7 +1183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7EC624-B5B6-46EE-84B1-DF9F4080EB6C}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1060,73 +1231,6 @@
       </c>
       <c r="B4" s="3">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DA93E-1B9C-4113-B4A9-8115F889330E}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1300,7 +1404,7 @@
     <row r="3" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>YWHS</v>
+        <v>ZWJD</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>75</v>
@@ -1312,7 +1416,7 @@
     <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>CWLA</v>
+        <v>FSHU</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>78</v>
@@ -1324,7 +1428,7 @@
     <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>YLCP</v>
+        <v>BRAW</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>76</v>
@@ -1336,7 +1440,7 @@
     <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PAMS</v>
+        <v>XVYX</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>75</v>
@@ -1348,7 +1452,7 @@
     <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>XXOL</v>
+        <v>HOUS</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>78</v>
@@ -1360,7 +1464,7 @@
     <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>CYAX</v>
+        <v>UASY</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>76</v>
@@ -1372,7 +1476,7 @@
     <row r="9" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>XUWB</v>
+        <v>XCWT</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>75</v>
@@ -1384,7 +1488,7 @@
     <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>UKBZ</v>
+        <v>WYEJ</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>78</v>
@@ -1655,6 +1759,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CE00FC-F1BA-4EE1-A3DF-8AB843E09614}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476F5C88-0CAA-4005-9A01-27383EE413C1}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -1693,7 +1860,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052181FB-1E4F-4A1E-B12D-45458B6E9387}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -1900,7 +2067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBF7BFE-850B-4F98-B614-3DDD73343798}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2002,7 +2169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E09210A-B3C7-4006-9111-ED419D27687A}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2351,7 +2518,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14030B2-06E1-4909-9E18-47749C3436A8}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2406,7 +2573,7 @@
     <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>TWJG</v>
+        <v>DJDD</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>80</v>
@@ -2421,7 +2588,7 @@
     <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>RRMI</v>
+        <v>ALQF</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>81</v>
@@ -2436,7 +2603,7 @@
     <row r="5" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WAUB</v>
+        <v>VHGL</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
@@ -2451,7 +2618,7 @@
     <row r="6" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ROKK</v>
+        <v>TIWK</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>80</v>
@@ -2466,7 +2633,7 @@
     <row r="7" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KDOI</v>
+        <v>FNUW</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>81</v>
@@ -2481,7 +2648,7 @@
     <row r="8" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>EWBX</v>
+        <v>PSMJ</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -2496,7 +2663,7 @@
     <row r="9" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>TOHJ</v>
+        <v>QFBF</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>80</v>
@@ -2511,7 +2678,7 @@
     <row r="10" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>WZGI</v>
+        <v>UDYT</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>81</v>
@@ -2528,7 +2695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA7453C-C911-4FD1-9109-F66FBE59E42C}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2558,7 +2725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA71A04-11EA-4D0B-B6D2-7FD344989619}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2605,7 +2772,7 @@
       </c>
       <c r="B3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>LASS</v>
+        <v>GWML</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -2617,7 +2784,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f t="shared" ref="B4:B11" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>NJRA</v>
+        <v>OWTJ</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -2629,7 +2796,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JKKS</v>
+        <v>WZDC</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -2641,7 +2808,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KFDC</v>
+        <v>NCIX</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -2653,7 +2820,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NRVY</v>
+        <v>SEOS</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -2665,7 +2832,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SCJM</v>
+        <v>JZDL</v>
       </c>
       <c r="C8" s="1">
         <v>7</v>
@@ -2677,7 +2844,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>HYBB</v>
+        <v>REXX</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
@@ -2689,7 +2856,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DBCT</v>
+        <v>GCHC</v>
       </c>
       <c r="C10" s="1">
         <v>9</v>
@@ -2701,47 +2868,10 @@
       </c>
       <c r="B11" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>LWFE</v>
+        <v>JCZR</v>
       </c>
       <c r="C11" s="1">
         <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD2043-75FB-4D5F-9033-C3F3EE0DCB0F}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement eMember SQL scripts management and enhance menu details page
- Introduced server actions for managing eMember SQL scripts, including fetching, adding, updating, and deleting scripts with error handling.
- Added `EmSqlScriptSchema` for validating SQL script submissions.
- Updated `SingleMenuPage` to integrate new components for displaying eMember menu details, including scripts, user guides, and tables.
- Created new components for managing SQL scripts, including `EmScripts`, `EmScriptForm`, `EmUserGuide`, and `EmMenuTables`.
- Enhanced UI with structured tabbed navigation and improved loading states for better user experience.
- Updated database schema to accommodate new SQL script management features.
</commit_message>
<xml_diff>
--- a/settings/Seed Data.xlsx
+++ b/settings/Seed Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XSP Project\xps-master-by-jk\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1059208A-7854-4702-9B99-11AB66C73732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614D4503-DC55-486C-8FE5-AF6EF7BB785A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Xps Test Cases" sheetId="7" r:id="rId1"/>
@@ -974,8 +974,8 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -983,13 +983,13 @@
     <col min="1" max="1" width="13.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" style="10" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="12" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" style="10" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" style="10" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" style="10" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" style="10" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="12" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
@@ -1003,7 +1003,7 @@
       <c r="C1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="9" t="s">
@@ -1021,7 +1021,7 @@
       <c r="I1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       <c r="C2" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -1044,7 +1044,7 @@
       <c r="F2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       <c r="C3" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="12" t="s">
         <v>81</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -1067,7 +1067,7 @@
       <c r="F3" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="12">
         <v>2</v>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       <c r="C4" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="12" t="s">
         <v>80</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -1090,7 +1090,7 @@
       <c r="F4" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="12">
         <v>3</v>
       </c>
     </row>
@@ -1104,7 +1104,7 @@
       <c r="C5" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="12" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="10" t="s">
@@ -1113,7 +1113,7 @@
       <c r="F5" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="12">
         <v>4</v>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       <c r="C6" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="12" t="s">
         <v>81</v>
       </c>
       <c r="E6" s="10" t="s">
@@ -1136,7 +1136,7 @@
       <c r="F6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="12">
         <v>5</v>
       </c>
     </row>
@@ -1404,7 +1404,7 @@
     <row r="3" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>ZWJD</v>
+        <v>TFTS</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>75</v>
@@ -1416,7 +1416,7 @@
     <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>FSHU</v>
+        <v>YYJT</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>78</v>
@@ -1428,7 +1428,7 @@
     <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>BRAW</v>
+        <v>AXRG</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>76</v>
@@ -1440,7 +1440,7 @@
     <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>XVYX</v>
+        <v>VBSP</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>75</v>
@@ -1452,7 +1452,7 @@
     <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>HOUS</v>
+        <v>HWHB</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>78</v>
@@ -1464,7 +1464,7 @@
     <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>UASY</v>
+        <v>KULJ</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>76</v>
@@ -1476,7 +1476,7 @@
     <row r="9" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>XCWT</v>
+        <v>QALE</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>75</v>
@@ -1488,7 +1488,7 @@
     <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>WYEJ</v>
+        <v>EVZU</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>78</v>
@@ -1765,7 +1765,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2573,7 +2573,7 @@
     <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>DJDD</v>
+        <v>XAJF</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>80</v>
@@ -2588,7 +2588,7 @@
     <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>ALQF</v>
+        <v>TPVI</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>81</v>
@@ -2603,7 +2603,7 @@
     <row r="5" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>VHGL</v>
+        <v>HTOF</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
@@ -2618,7 +2618,7 @@
     <row r="6" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>TIWK</v>
+        <v>OLXP</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>80</v>
@@ -2633,7 +2633,7 @@
     <row r="7" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>FNUW</v>
+        <v>VRPM</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>81</v>
@@ -2648,7 +2648,7 @@
     <row r="8" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PSMJ</v>
+        <v>SZYM</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -2663,7 +2663,7 @@
     <row r="9" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>QFBF</v>
+        <v>GQVY</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>80</v>
@@ -2678,7 +2678,7 @@
     <row r="10" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>UDYT</v>
+        <v>XZGM</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>81</v>
@@ -2772,7 +2772,7 @@
       </c>
       <c r="B3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>GWML</v>
+        <v>ZSYW</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -2784,7 +2784,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f t="shared" ref="B4:B11" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>OWTJ</v>
+        <v>XCPT</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -2796,7 +2796,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>WZDC</v>
+        <v>DFBQ</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -2808,7 +2808,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>NCIX</v>
+        <v>GOLV</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -2820,7 +2820,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SEOS</v>
+        <v>JAGY</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -2832,7 +2832,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JZDL</v>
+        <v>TNAM</v>
       </c>
       <c r="C8" s="1">
         <v>7</v>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>REXX</v>
+        <v>YLUE</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>GCHC</v>
+        <v>PDTR</v>
       </c>
       <c r="C10" s="1">
         <v>9</v>
@@ -2868,7 +2868,7 @@
       </c>
       <c r="B11" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JCZR</v>
+        <v>FLQQ</v>
       </c>
       <c r="C11" s="1">
         <v>9</v>

</xml_diff>

<commit_message>
Add eMember and XPS Released Tasks management actions and UI components
- Introduced server actions for managing eMember and XPS Released Tasks, including fetching, adding, updating, and deleting tasks with error handling.
- Created `EmRTColumns`, `XpsRTColumns`, and respective form components for structured UI and task management.
- Integrated `XpsRTFormSchema` for validating task submissions.
- Enhanced user interaction with improved loading states and error handling across components.
- Updated the schema to accommodate new task management features.
</commit_message>
<xml_diff>
--- a/settings/Seed Data.xlsx
+++ b/settings/Seed Data.xlsx
@@ -8,25 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\XSP Project\xps-master-by-jk\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614D4503-DC55-486C-8FE5-AF6EF7BB785A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1276087D-C94C-4FC8-ADC7-5C57B90DB5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="879" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Xps Test Cases" sheetId="7" r:id="rId1"/>
-    <sheet name="eMember Columns" sheetId="13" r:id="rId2"/>
-    <sheet name="eMember Tables" sheetId="2" r:id="rId3"/>
-    <sheet name="Enum" sheetId="19" r:id="rId4"/>
-    <sheet name="Portals" sheetId="17" r:id="rId5"/>
-    <sheet name="Users" sheetId="18" r:id="rId6"/>
-    <sheet name="Xps Menu" sheetId="6" r:id="rId7"/>
-    <sheet name="Xps Menu Descriptions" sheetId="4" r:id="rId8"/>
-    <sheet name="Xps User Guide" sheetId="5" r:id="rId9"/>
-    <sheet name="Xps Tables" sheetId="3" r:id="rId10"/>
-    <sheet name="Xps Columns" sheetId="8" r:id="rId11"/>
-    <sheet name="Xps Bugs" sheetId="9" r:id="rId12"/>
-    <sheet name="Xps Released Task" sheetId="10" r:id="rId13"/>
-    <sheet name="eMember Menu" sheetId="11" r:id="rId14"/>
+    <sheet name="Enum" sheetId="19" r:id="rId1"/>
+    <sheet name="Portals" sheetId="17" r:id="rId2"/>
+    <sheet name="Users" sheetId="18" r:id="rId3"/>
+    <sheet name="Xps Menu" sheetId="6" r:id="rId4"/>
+    <sheet name="Xps Test Cases" sheetId="7" r:id="rId5"/>
+    <sheet name="Xps Menu Descriptions" sheetId="4" r:id="rId6"/>
+    <sheet name="Xps User Guide" sheetId="5" r:id="rId7"/>
+    <sheet name="Xps Tables" sheetId="3" r:id="rId8"/>
+    <sheet name="Xps Columns" sheetId="8" r:id="rId9"/>
+    <sheet name="Xps Bugs" sheetId="9" r:id="rId10"/>
+    <sheet name="Xps Released Task" sheetId="10" r:id="rId11"/>
+    <sheet name="eMember Menu" sheetId="11" r:id="rId12"/>
+    <sheet name="eMember Tables" sheetId="2" r:id="rId13"/>
+    <sheet name="eMember Columns" sheetId="13" r:id="rId14"/>
     <sheet name="eMember Menu Desc" sheetId="12" r:id="rId15"/>
     <sheet name="eMember User Guide" sheetId="1" r:id="rId16"/>
     <sheet name="eMember Test Cases" sheetId="14" r:id="rId17"/>
@@ -968,277 +968,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DA93E-1B9C-4113-B4A9-8115F889330E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052181FB-1E4F-4A1E-B12D-45458B6E9387}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="16.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="14.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>12</v>
+        <v>82</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>158</v>
+        <v>74</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>159</v>
+        <v>20</v>
       </c>
       <c r="C2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C3" s="10" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="10" t="s">
+    </row>
+    <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="J3" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="D5" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="J4" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="D6" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="J5" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="12">
-        <v>5</v>
+      <c r="I6" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD2043-75FB-4D5F-9033-C3F3EE0DCB0F}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7EC624-B5B6-46EE-84B1-DF9F4080EB6C}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A989FAC-8575-4264-86E5-883569E54F3F}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1297,7 +1233,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBFE0B6-E602-4629-B2D2-1D3D79579B76}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1356,14 +1292,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F88E74-BD67-42CE-B055-DDE648DF10E9}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1404,7 +1340,7 @@
     <row r="3" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>TFTS</v>
+        <v>QRCX</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>75</v>
@@ -1416,7 +1352,7 @@
     <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>YYJT</v>
+        <v>VJCC</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>78</v>
@@ -1428,7 +1364,7 @@
     <row r="5" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>AXRG</v>
+        <v>JMHU</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>76</v>
@@ -1440,7 +1376,7 @@
     <row r="6" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>VBSP</v>
+        <v>RRRD</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>75</v>
@@ -1452,7 +1388,7 @@
     <row r="7" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>HWHB</v>
+        <v>QFGR</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>78</v>
@@ -1464,7 +1400,7 @@
     <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>KULJ</v>
+        <v>LEDM</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>76</v>
@@ -1476,7 +1412,7 @@
     <row r="9" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>QALE</v>
+        <v>KTOS</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>75</v>
@@ -1488,13 +1424,115 @@
     <row r="10" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>EVZU</v>
+        <v>VONK</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476F5C88-0CAA-4005-9A01-27383EE413C1}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CE00FC-F1BA-4EE1-A3DF-8AB843E09614}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1759,315 +1797,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CE00FC-F1BA-4EE1-A3DF-8AB843E09614}">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B2" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{476F5C88-0CAA-4005-9A01-27383EE413C1}">
-  <sheetPr>
-    <tabColor rgb="FF00B0F0"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="26.42578125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.42578125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{052181FB-1E4F-4A1E-B12D-45458B6E9387}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="14.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="10"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBF7BFE-850B-4F98-B614-3DDD73343798}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2169,7 +1898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E09210A-B3C7-4006-9111-ED419D27687A}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -2518,7 +2247,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14030B2-06E1-4909-9E18-47749C3436A8}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2573,7 +2302,7 @@
     <row r="3" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>XAJF</v>
+        <v>IIVA</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>80</v>
@@ -2588,7 +2317,7 @@
     <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="str">
         <f t="shared" ref="A4:A9" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>TPVI</v>
+        <v>MWBZ</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>81</v>
@@ -2603,7 +2332,7 @@
     <row r="5" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>HTOF</v>
+        <v>RNHQ</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
@@ -2618,7 +2347,7 @@
     <row r="6" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>OLXP</v>
+        <v>FJKN</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>80</v>
@@ -2633,7 +2362,7 @@
     <row r="7" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>VRPM</v>
+        <v>GVZP</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>81</v>
@@ -2648,7 +2377,7 @@
     <row r="8" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>SZYM</v>
+        <v>HNTJ</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>20</v>
@@ -2663,7 +2392,7 @@
     <row r="9" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>GQVY</v>
+        <v>FVFU</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>80</v>
@@ -2678,7 +2407,7 @@
     <row r="10" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>XZGM</v>
+        <v>EOAR</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>81</v>
@@ -2695,7 +2424,186 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82DA93E-1B9C-4113-B4A9-8115F889330E}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="10" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" style="10" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="12" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="J5" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="12">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA7453C-C911-4FD1-9109-F66FBE59E42C}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2725,7 +2633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA71A04-11EA-4D0B-B6D2-7FD344989619}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2772,7 +2680,7 @@
       </c>
       <c r="B3" s="3" t="str">
         <f ca="1">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>ZSYW</v>
+        <v>TJIJ</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -2784,7 +2692,7 @@
       </c>
       <c r="B4" s="3" t="str">
         <f t="shared" ref="B4:B11" ca="1" si="0">CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))</f>
-        <v>XCPT</v>
+        <v>BYDT</v>
       </c>
       <c r="C4" s="1">
         <v>3</v>
@@ -2796,7 +2704,7 @@
       </c>
       <c r="B5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>DFBQ</v>
+        <v>OKUX</v>
       </c>
       <c r="C5" s="1">
         <v>4</v>
@@ -2808,7 +2716,7 @@
       </c>
       <c r="B6" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>GOLV</v>
+        <v>KZQY</v>
       </c>
       <c r="C6" s="1">
         <v>5</v>
@@ -2820,7 +2728,7 @@
       </c>
       <c r="B7" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>JAGY</v>
+        <v>ZJKX</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -2832,7 +2740,7 @@
       </c>
       <c r="B8" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>TNAM</v>
+        <v>IUQJ</v>
       </c>
       <c r="C8" s="1">
         <v>7</v>
@@ -2844,7 +2752,7 @@
       </c>
       <c r="B9" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>YLUE</v>
+        <v>HWQD</v>
       </c>
       <c r="C9" s="1">
         <v>8</v>
@@ -2856,7 +2764,7 @@
       </c>
       <c r="B10" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>PDTR</v>
+        <v>LJOF</v>
       </c>
       <c r="C10" s="1">
         <v>9</v>
@@ -2868,10 +2776,102 @@
       </c>
       <c r="B11" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>FLQQ</v>
+        <v>ZMUX</v>
       </c>
       <c r="C11" s="1">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BD2043-75FB-4D5F-9033-C3F3EE0DCB0F}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7EC624-B5B6-46EE-84B1-DF9F4080EB6C}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>